<commit_message>
KP-303 add map data
</commit_message>
<xml_diff>
--- a/Documents/Lコース座標.xlsx
+++ b/Documents/Lコース座標.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KaoruOta/ET_Robocon/ev3rt-beta7-release/hrp2/sdk/workspace/hiro_jiren/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{3758D16D-B1A8-9144-B59F-649E7E02C97C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{8D893AED-2C4C-924D-9687-487A9416336F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3300" yWindow="460" windowWidth="35100" windowHeight="21140" activeTab="5" xr2:uid="{6DB03CC7-F739-074A-9B67-9A070117031E}"/>
+    <workbookView xWindow="21060" yWindow="460" windowWidth="16380" windowHeight="21140" activeTab="12" xr2:uid="{6DB03CC7-F739-074A-9B67-9A070117031E}"/>
   </bookViews>
   <sheets>
     <sheet name="Start-1st_CR" sheetId="1" r:id="rId1"/>
@@ -25,8 +25,14 @@
     <sheet name="走行コンセプト①" sheetId="11" r:id="rId10"/>
     <sheet name="走行コンセプト②" sheetId="12" r:id="rId11"/>
     <sheet name="走行コンセプト③" sheetId="13" r:id="rId12"/>
-    <sheet name="Sheet3" sheetId="15" r:id="rId13"/>
+    <sheet name="ブロックビンコ" sheetId="15" r:id="rId13"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">ブロックビンコ!$P$2</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">ブロックビンコ!$P$3:$P$32</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">ブロックビンコ!$Q$2</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">ブロックビンコ!$Q$3:$Q$32</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,9 +43,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
   <si>
     <t>ß</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>y</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -47,6 +67,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="0_ "/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="12"/>
@@ -72,7 +95,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -95,17 +118,127 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -123,6 +256,997 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ja-JP"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ブロックビンコ!$Q$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>y</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>ブロックビンコ!$P$3:$P$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>525</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>875</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1225</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>525</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1225</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>525</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>875</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1225</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1400</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>ブロックビンコ!$Q$3:$Q$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1225</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1225</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1225</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>875</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>875</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>525</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>525</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>525</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>350</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5533-3647-8A15-EB4BF32DBB78}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1424714687"/>
+        <c:axId val="1425471199"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1424714687"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1425471199"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1425471199"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1424714687"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ja-JP"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5596,13 +6720,13 @@
     <xdr:from>
       <xdr:col>92</xdr:col>
       <xdr:colOff>317500</xdr:colOff>
-      <xdr:row>212</xdr:row>
+      <xdr:row>131</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>94</xdr:col>
       <xdr:colOff>317500</xdr:colOff>
-      <xdr:row>220</xdr:row>
+      <xdr:row>139</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5618,7 +6742,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="93789500" y="53975000"/>
+          <a:off x="93789500" y="33401000"/>
           <a:ext cx="2032000" cy="2032000"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -5657,16 +6781,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>83</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>87</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>97</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>91</xdr:col>
-      <xdr:colOff>698500</xdr:colOff>
-      <xdr:row>114</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>825500</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5681,7 +6805,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="88544400" y="24663400"/>
+          <a:off x="84607400" y="21996400"/>
           <a:ext cx="4610100" cy="4292600"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -6059,15 +7183,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>90</xdr:col>
-      <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>111</xdr:row>
+      <xdr:col>81</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>89</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>92</xdr:col>
-      <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>119</xdr:row>
+      <xdr:col>83</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>97</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6083,7 +7207,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="92163900" y="28219400"/>
+          <a:off x="82384900" y="22631400"/>
           <a:ext cx="2032000" cy="2032000"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -6118,6 +7242,124 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>97</xdr:col>
+      <xdr:colOff>299788</xdr:colOff>
+      <xdr:row>209</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>108</xdr:col>
+      <xdr:colOff>591888</xdr:colOff>
+      <xdr:row>226</xdr:row>
+      <xdr:rowOff>207400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="52" name="正方形/長方形 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFAF1629-2914-0F48-B9E4-B2571A795C80}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="98851788" y="53111400"/>
+          <a:ext cx="11468100" cy="4500000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="17000">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>(2495,2075)</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="17000">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>876300</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="グラフ 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B95F73ED-2A03-2740-8BC7-F25252F2C538}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -18144,8 +19386,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB0DD1CD-4FA4-9E45-B6BB-0F24850E37CC}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A80" zoomScale="10" zoomScaleNormal="10" workbookViewId="0">
-      <selection activeCell="EL301" sqref="EL301"/>
+    <sheetView topLeftCell="A79" zoomScale="10" zoomScaleNormal="10" workbookViewId="0">
+      <selection activeCell="EP231" sqref="EP231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -18158,46 +19400,861 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC0D6C9E-10A1-E446-929B-01BD39C51451}">
-  <dimension ref="E6:E10"/>
+  <dimension ref="C1:Q32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="O16" zoomScale="186" zoomScaleNormal="186" workbookViewId="0">
+      <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
   <sheetData>
-    <row r="6" spans="5:5">
+    <row r="1" spans="3:17" ht="21" thickBot="1"/>
+    <row r="2" spans="3:17">
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" s="3"/>
+      <c r="P2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="3:17">
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <f>C3*350</f>
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>1050</v>
+      </c>
+      <c r="I3">
+        <v>350</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>1050</v>
+      </c>
+      <c r="O3" s="6">
+        <v>0</v>
+      </c>
+      <c r="P3" s="7">
+        <f>L3+350</f>
+        <v>350</v>
+      </c>
+      <c r="Q3" s="8">
+        <f>M3+350</f>
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="4" spans="3:17">
+      <c r="C4">
+        <f>C3+1</f>
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D6" si="0">C4*350</f>
+        <v>350</v>
+      </c>
+      <c r="E4">
+        <v>1050</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>350</v>
+      </c>
+      <c r="M4">
+        <v>1050</v>
+      </c>
+      <c r="O4" s="6">
+        <v>1</v>
+      </c>
+      <c r="P4" s="7">
+        <f t="shared" ref="P4:P6" si="1">L4+350</f>
+        <v>700</v>
+      </c>
+      <c r="Q4" s="8">
+        <f t="shared" ref="Q4:Q6" si="2">M4+350</f>
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="5" spans="3:17">
+      <c r="C5">
+        <f t="shared" ref="C5:C6" si="3">C4+1</f>
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>700</v>
+      </c>
+      <c r="E5">
+        <v>1050</v>
+      </c>
+      <c r="I5">
+        <f>I3/I4</f>
+        <v>175</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <v>700</v>
+      </c>
+      <c r="M5">
+        <v>1050</v>
+      </c>
+      <c r="O5" s="6">
+        <v>2</v>
+      </c>
+      <c r="P5" s="7">
+        <f t="shared" si="1"/>
+        <v>1050</v>
+      </c>
+      <c r="Q5" s="8">
+        <f t="shared" si="2"/>
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="6" spans="3:17">
+      <c r="C6">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>1050</v>
+      </c>
       <c r="E6">
-        <v>1335</v>
+        <v>1050</v>
+      </c>
+      <c r="I6">
+        <f>SQRT(2)</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="K6">
+        <v>3</v>
+      </c>
+      <c r="L6">
+        <v>1050</v>
+      </c>
+      <c r="M6">
+        <v>1050</v>
+      </c>
+      <c r="O6" s="6">
+        <v>3</v>
+      </c>
+      <c r="P6" s="7">
+        <f t="shared" si="1"/>
+        <v>1400</v>
+      </c>
+      <c r="Q6" s="8">
+        <f t="shared" si="2"/>
+        <v>1400</v>
       </c>
     </row>
-    <row r="7" spans="5:5">
-      <c r="E7">
-        <v>1075</v>
-      </c>
+    <row r="7" spans="3:17" ht="23" customHeight="1">
+      <c r="I7">
+        <f>I5*I6</f>
+        <v>247.48737341529164</v>
+      </c>
+      <c r="O7" s="6"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="8"/>
     </row>
-    <row r="8" spans="5:5">
-      <c r="E8">
-        <f>E6-E7</f>
-        <v>260</v>
+    <row r="8" spans="3:17">
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8" s="2">
+        <v>175</v>
+      </c>
+      <c r="E8" s="2">
+        <f>E17+350</f>
+        <v>875</v>
+      </c>
+      <c r="K8">
+        <v>4</v>
+      </c>
+      <c r="L8">
+        <v>175</v>
+      </c>
+      <c r="M8">
+        <v>875</v>
+      </c>
+      <c r="O8" s="6">
+        <v>4</v>
+      </c>
+      <c r="P8" s="7">
+        <f t="shared" ref="P8:P10" si="4">L8+350</f>
+        <v>525</v>
+      </c>
+      <c r="Q8" s="8">
+        <f t="shared" ref="Q8:Q10" si="5">M8+350</f>
+        <v>1225</v>
       </c>
     </row>
-    <row r="9" spans="5:5">
+    <row r="9" spans="3:17">
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9" s="2">
+        <v>525</v>
+      </c>
       <c r="E9">
-        <f>E8/2</f>
-        <v>130</v>
+        <v>875</v>
+      </c>
+      <c r="K9">
+        <v>5</v>
+      </c>
+      <c r="L9">
+        <v>525</v>
+      </c>
+      <c r="M9">
+        <v>875</v>
+      </c>
+      <c r="O9" s="6">
+        <v>5</v>
+      </c>
+      <c r="P9" s="7">
+        <f t="shared" si="4"/>
+        <v>875</v>
+      </c>
+      <c r="Q9" s="8">
+        <f t="shared" si="5"/>
+        <v>1225</v>
       </c>
     </row>
-    <row r="10" spans="5:5">
+    <row r="10" spans="3:17">
+      <c r="C10">
+        <v>6</v>
+      </c>
+      <c r="D10" s="2">
+        <v>875</v>
+      </c>
       <c r="E10">
-        <f>E7+E9</f>
-        <v>1205</v>
+        <v>875</v>
+      </c>
+      <c r="K10">
+        <v>6</v>
+      </c>
+      <c r="L10">
+        <v>875</v>
+      </c>
+      <c r="M10">
+        <v>875</v>
+      </c>
+      <c r="O10" s="6">
+        <v>6</v>
+      </c>
+      <c r="P10" s="7">
+        <f t="shared" si="4"/>
+        <v>1225</v>
+      </c>
+      <c r="Q10" s="8">
+        <f t="shared" si="5"/>
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="11" spans="3:17">
+      <c r="O11" s="6"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="8"/>
+    </row>
+    <row r="12" spans="3:17">
+      <c r="C12">
+        <f>C10+1</f>
+        <v>7</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>700</v>
+      </c>
+      <c r="K12">
+        <v>7</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>700</v>
+      </c>
+      <c r="O12" s="6">
+        <v>7</v>
+      </c>
+      <c r="P12" s="7">
+        <f t="shared" ref="P12:P15" si="6">L12+350</f>
+        <v>350</v>
+      </c>
+      <c r="Q12" s="8">
+        <f t="shared" ref="Q12:Q15" si="7">M12+350</f>
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="13" spans="3:17">
+      <c r="C13">
+        <f>C12+1</f>
+        <v>8</v>
+      </c>
+      <c r="D13">
+        <v>350</v>
+      </c>
+      <c r="E13">
+        <v>700</v>
+      </c>
+      <c r="K13">
+        <v>8</v>
+      </c>
+      <c r="L13">
+        <v>350</v>
+      </c>
+      <c r="M13">
+        <v>700</v>
+      </c>
+      <c r="O13" s="6">
+        <v>8</v>
+      </c>
+      <c r="P13" s="7">
+        <f t="shared" si="6"/>
+        <v>700</v>
+      </c>
+      <c r="Q13" s="8">
+        <f t="shared" si="7"/>
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="14" spans="3:17">
+      <c r="C14">
+        <f t="shared" ref="C14:C15" si="8">C13+1</f>
+        <v>9</v>
+      </c>
+      <c r="D14">
+        <v>700</v>
+      </c>
+      <c r="E14">
+        <v>700</v>
+      </c>
+      <c r="K14">
+        <v>9</v>
+      </c>
+      <c r="L14">
+        <v>700</v>
+      </c>
+      <c r="M14">
+        <v>700</v>
+      </c>
+      <c r="O14" s="6">
+        <v>9</v>
+      </c>
+      <c r="P14" s="7">
+        <f t="shared" si="6"/>
+        <v>1050</v>
+      </c>
+      <c r="Q14" s="8">
+        <f t="shared" si="7"/>
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="15" spans="3:17">
+      <c r="C15">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="D15">
+        <v>1050</v>
+      </c>
+      <c r="E15">
+        <v>700</v>
+      </c>
+      <c r="K15">
+        <v>10</v>
+      </c>
+      <c r="L15">
+        <v>1050</v>
+      </c>
+      <c r="M15">
+        <v>700</v>
+      </c>
+      <c r="O15" s="6">
+        <v>10</v>
+      </c>
+      <c r="P15" s="7">
+        <f t="shared" si="6"/>
+        <v>1400</v>
+      </c>
+      <c r="Q15" s="8">
+        <f t="shared" si="7"/>
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="16" spans="3:17">
+      <c r="O16" s="6"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="8"/>
+    </row>
+    <row r="17" spans="3:17">
+      <c r="C17">
+        <f>C15+1</f>
+        <v>11</v>
+      </c>
+      <c r="D17" s="2">
+        <v>175</v>
+      </c>
+      <c r="E17" s="2">
+        <f>D17+350</f>
+        <v>525</v>
+      </c>
+      <c r="K17">
+        <v>11</v>
+      </c>
+      <c r="L17">
+        <v>175</v>
+      </c>
+      <c r="M17">
+        <v>525</v>
+      </c>
+      <c r="O17" s="6">
+        <v>11</v>
+      </c>
+      <c r="P17" s="7">
+        <f t="shared" ref="P17:P18" si="9">L17+350</f>
+        <v>525</v>
+      </c>
+      <c r="Q17" s="8">
+        <f t="shared" ref="Q17:Q18" si="10">M17+350</f>
+        <v>875</v>
+      </c>
+    </row>
+    <row r="18" spans="3:17">
+      <c r="C18">
+        <f>C17+1</f>
+        <v>12</v>
+      </c>
+      <c r="D18" s="2">
+        <v>875</v>
+      </c>
+      <c r="E18" s="2">
+        <v>525</v>
+      </c>
+      <c r="K18">
+        <v>12</v>
+      </c>
+      <c r="L18">
+        <v>875</v>
+      </c>
+      <c r="M18">
+        <v>525</v>
+      </c>
+      <c r="O18" s="6">
+        <v>12</v>
+      </c>
+      <c r="P18" s="7">
+        <f t="shared" si="9"/>
+        <v>1225</v>
+      </c>
+      <c r="Q18" s="8">
+        <f t="shared" si="10"/>
+        <v>875</v>
+      </c>
+    </row>
+    <row r="19" spans="3:17">
+      <c r="O19" s="6"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="8"/>
+    </row>
+    <row r="20" spans="3:17">
+      <c r="C20">
+        <f>C18+1</f>
+        <v>13</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>350</v>
+      </c>
+      <c r="K20">
+        <v>13</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>350</v>
+      </c>
+      <c r="O20" s="6">
+        <v>13</v>
+      </c>
+      <c r="P20" s="7">
+        <f t="shared" ref="P20:P23" si="11">L20+350</f>
+        <v>350</v>
+      </c>
+      <c r="Q20" s="8">
+        <f t="shared" ref="Q20:Q23" si="12">M20+350</f>
+        <v>700</v>
+      </c>
+    </row>
+    <row r="21" spans="3:17">
+      <c r="C21">
+        <f>C20+1</f>
+        <v>14</v>
+      </c>
+      <c r="D21">
+        <v>350</v>
+      </c>
+      <c r="E21">
+        <v>350</v>
+      </c>
+      <c r="K21">
+        <v>14</v>
+      </c>
+      <c r="L21">
+        <v>350</v>
+      </c>
+      <c r="M21">
+        <v>350</v>
+      </c>
+      <c r="O21" s="6">
+        <v>14</v>
+      </c>
+      <c r="P21" s="7">
+        <f t="shared" si="11"/>
+        <v>700</v>
+      </c>
+      <c r="Q21" s="8">
+        <f t="shared" si="12"/>
+        <v>700</v>
+      </c>
+    </row>
+    <row r="22" spans="3:17">
+      <c r="C22">
+        <f t="shared" ref="C22:C23" si="13">C21+1</f>
+        <v>15</v>
+      </c>
+      <c r="D22">
+        <v>700</v>
+      </c>
+      <c r="E22">
+        <v>350</v>
+      </c>
+      <c r="K22">
+        <v>15</v>
+      </c>
+      <c r="L22">
+        <v>700</v>
+      </c>
+      <c r="M22">
+        <v>350</v>
+      </c>
+      <c r="O22" s="6">
+        <v>15</v>
+      </c>
+      <c r="P22" s="7">
+        <f t="shared" si="11"/>
+        <v>1050</v>
+      </c>
+      <c r="Q22" s="8">
+        <f t="shared" si="12"/>
+        <v>700</v>
+      </c>
+    </row>
+    <row r="23" spans="3:17">
+      <c r="C23">
+        <f t="shared" si="13"/>
+        <v>16</v>
+      </c>
+      <c r="D23">
+        <v>1050</v>
+      </c>
+      <c r="E23">
+        <v>350</v>
+      </c>
+      <c r="K23">
+        <v>16</v>
+      </c>
+      <c r="L23">
+        <v>1050</v>
+      </c>
+      <c r="M23">
+        <v>350</v>
+      </c>
+      <c r="O23" s="6">
+        <v>16</v>
+      </c>
+      <c r="P23" s="7">
+        <f t="shared" si="11"/>
+        <v>1400</v>
+      </c>
+      <c r="Q23" s="8">
+        <f t="shared" si="12"/>
+        <v>700</v>
+      </c>
+    </row>
+    <row r="24" spans="3:17">
+      <c r="O24" s="6"/>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="8"/>
+    </row>
+    <row r="25" spans="3:17">
+      <c r="C25">
+        <f>C23+1</f>
+        <v>17</v>
+      </c>
+      <c r="D25" s="2">
+        <v>175</v>
+      </c>
+      <c r="E25" s="2">
+        <v>175</v>
+      </c>
+      <c r="K25">
+        <v>17</v>
+      </c>
+      <c r="L25">
+        <v>175</v>
+      </c>
+      <c r="M25">
+        <v>175</v>
+      </c>
+      <c r="O25" s="6">
+        <v>17</v>
+      </c>
+      <c r="P25" s="7">
+        <f t="shared" ref="P25:P27" si="14">L25+350</f>
+        <v>525</v>
+      </c>
+      <c r="Q25" s="8">
+        <f t="shared" ref="Q25:Q27" si="15">M25+350</f>
+        <v>525</v>
+      </c>
+    </row>
+    <row r="26" spans="3:17">
+      <c r="C26">
+        <f>C25+1</f>
+        <v>18</v>
+      </c>
+      <c r="D26" s="2">
+        <f>D25+350</f>
+        <v>525</v>
+      </c>
+      <c r="E26" s="2">
+        <v>175</v>
+      </c>
+      <c r="K26">
+        <v>18</v>
+      </c>
+      <c r="L26">
+        <v>525</v>
+      </c>
+      <c r="M26">
+        <v>175</v>
+      </c>
+      <c r="O26" s="6">
+        <v>18</v>
+      </c>
+      <c r="P26" s="7">
+        <f t="shared" si="14"/>
+        <v>875</v>
+      </c>
+      <c r="Q26" s="8">
+        <f t="shared" si="15"/>
+        <v>525</v>
+      </c>
+    </row>
+    <row r="27" spans="3:17">
+      <c r="C27">
+        <f>C26+1</f>
+        <v>19</v>
+      </c>
+      <c r="D27" s="2">
+        <f>D26+350</f>
+        <v>875</v>
+      </c>
+      <c r="E27" s="2">
+        <v>175</v>
+      </c>
+      <c r="K27">
+        <v>19</v>
+      </c>
+      <c r="L27">
+        <v>875</v>
+      </c>
+      <c r="M27">
+        <v>175</v>
+      </c>
+      <c r="O27" s="6">
+        <v>19</v>
+      </c>
+      <c r="P27" s="7">
+        <f t="shared" si="14"/>
+        <v>1225</v>
+      </c>
+      <c r="Q27" s="8">
+        <f t="shared" si="15"/>
+        <v>525</v>
+      </c>
+    </row>
+    <row r="28" spans="3:17">
+      <c r="O28" s="6"/>
+      <c r="P28" s="7"/>
+      <c r="Q28" s="8"/>
+    </row>
+    <row r="29" spans="3:17">
+      <c r="C29">
+        <f>C27+1</f>
+        <v>20</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>20</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <v>0</v>
+      </c>
+      <c r="O29" s="6">
+        <v>20</v>
+      </c>
+      <c r="P29" s="7">
+        <f t="shared" ref="P29:P32" si="16">L29+350</f>
+        <v>350</v>
+      </c>
+      <c r="Q29" s="8">
+        <f t="shared" ref="Q29:Q32" si="17">M29+350</f>
+        <v>350</v>
+      </c>
+    </row>
+    <row r="30" spans="3:17">
+      <c r="C30">
+        <f>C29+1</f>
+        <v>21</v>
+      </c>
+      <c r="D30">
+        <v>350</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <v>21</v>
+      </c>
+      <c r="L30">
+        <v>350</v>
+      </c>
+      <c r="M30">
+        <v>0</v>
+      </c>
+      <c r="O30" s="6">
+        <v>21</v>
+      </c>
+      <c r="P30" s="7">
+        <f t="shared" si="16"/>
+        <v>700</v>
+      </c>
+      <c r="Q30" s="8">
+        <f t="shared" si="17"/>
+        <v>350</v>
+      </c>
+    </row>
+    <row r="31" spans="3:17">
+      <c r="C31">
+        <f t="shared" ref="C31:C32" si="18">C30+1</f>
+        <v>22</v>
+      </c>
+      <c r="D31">
+        <v>700</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <v>22</v>
+      </c>
+      <c r="L31">
+        <v>700</v>
+      </c>
+      <c r="M31">
+        <v>0</v>
+      </c>
+      <c r="O31" s="6">
+        <v>22</v>
+      </c>
+      <c r="P31" s="7">
+        <f t="shared" si="16"/>
+        <v>1050</v>
+      </c>
+      <c r="Q31" s="8">
+        <f t="shared" si="17"/>
+        <v>350</v>
+      </c>
+    </row>
+    <row r="32" spans="3:17" ht="21" thickBot="1">
+      <c r="C32">
+        <f t="shared" si="18"/>
+        <v>23</v>
+      </c>
+      <c r="D32">
+        <v>1050</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <v>23</v>
+      </c>
+      <c r="L32">
+        <v>1050</v>
+      </c>
+      <c r="M32">
+        <v>0</v>
+      </c>
+      <c r="O32" s="9">
+        <v>23</v>
+      </c>
+      <c r="P32" s="10">
+        <f t="shared" si="16"/>
+        <v>1400</v>
+      </c>
+      <c r="Q32" s="11">
+        <f t="shared" si="17"/>
+        <v>350</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -18281,7 +20338,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2D3F457-5443-8140-A1C2-32A729A4C0D5}">
   <dimension ref="EI332"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="10" zoomScaleNormal="10" workbookViewId="0">
+    <sheetView topLeftCell="A99" zoomScale="10" zoomScaleNormal="10" workbookViewId="0">
       <selection activeCell="FQ248" sqref="FQ248"/>
     </sheetView>
   </sheetViews>

</xml_diff>